<commit_message>
new cue style and new data dir name
</commit_message>
<xml_diff>
--- a/dataAnalysisCodes/watchERP/01-preprocess-plot/watchErpDataset2.xlsx
+++ b/dataAnalysisCodes/watchERP/01-preprocess-plot/watchErpDataset2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="85">
   <si>
     <t>date</t>
   </si>
@@ -214,6 +214,63 @@
   </si>
   <si>
     <t>2013-02-28-marijn</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>2013-03-04-14-51-57</t>
+  </si>
+  <si>
+    <t>2013-03-04-15-00-40</t>
+  </si>
+  <si>
+    <t>2013-03-04-15-06-10</t>
+  </si>
+  <si>
+    <t>2013-03-04-15-12-15</t>
+  </si>
+  <si>
+    <t>2013-03-04-15-21-41</t>
+  </si>
+  <si>
+    <t>2013-03-04-15-34-23</t>
+  </si>
+  <si>
+    <t>2013-03-04-15-40-19</t>
+  </si>
+  <si>
+    <t>2013-03-04-15-46-20</t>
+  </si>
+  <si>
+    <t>2013-03-04-15-52-05</t>
+  </si>
+  <si>
+    <t>2013-03-04-15-58-31</t>
+  </si>
+  <si>
+    <t>2013-03-04-16-16-00</t>
+  </si>
+  <si>
+    <t>2013-03-04-16-21-35</t>
+  </si>
+  <si>
+    <t>2013-03-04-16-29-47</t>
+  </si>
+  <si>
+    <t>2013-03-04-16-36-52</t>
+  </si>
+  <si>
+    <t>2013-03-04-16-44-05</t>
+  </si>
+  <si>
+    <t>2013-03-04-nick</t>
+  </si>
+  <si>
+    <t>oddball.bdf</t>
   </si>
 </sst>
 </file>
@@ -569,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:A46"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,6 +1699,351 @@
         <v>46</v>
       </c>
       <c r="G46" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" s="3">
+        <v>41337</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G47" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C48" s="3">
+        <v>41337</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G48" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C49" s="3">
+        <v>41337</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G49" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C50" s="3">
+        <v>41337</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G50" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="3">
+        <v>41337</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G51" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" s="3">
+        <v>41337</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G52" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="3">
+        <v>41337</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G53" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C54" s="3">
+        <v>41337</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G54" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55" s="3">
+        <v>41337</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G55" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C56" s="3">
+        <v>41337</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G56" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="3">
+        <v>41337</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G57" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" s="3">
+        <v>41337</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G58" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C59" s="3">
+        <v>41337</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G59" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C60" s="3">
+        <v>41337</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G60" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61" s="3">
+        <v>41337</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G61" s="2">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding bayesian LDA classif
</commit_message>
<xml_diff>
--- a/dataAnalysisCodes/watchERP/01-preprocess-plot/watchErpDataset2.xlsx
+++ b/dataAnalysisCodes/watchERP/01-preprocess-plot/watchErpDataset2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="103">
   <si>
     <t>date</t>
   </si>
@@ -271,6 +271,60 @@
   </si>
   <si>
     <t>oddball.bdf</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>Jaime</t>
+  </si>
+  <si>
+    <t>2013-03-05-jaime</t>
+  </si>
+  <si>
+    <t>2013-03-05-16-22-01</t>
+  </si>
+  <si>
+    <t>2013-03-05-16-30-48</t>
+  </si>
+  <si>
+    <t>2013-03-05-16-38-38</t>
+  </si>
+  <si>
+    <t>2013-03-05-16-44-25</t>
+  </si>
+  <si>
+    <t>2013-03-05-16-51-03</t>
+  </si>
+  <si>
+    <t>2013-03-05-17-04-04</t>
+  </si>
+  <si>
+    <t>2013-03-05-17-09-20</t>
+  </si>
+  <si>
+    <t>2013-03-05-17-17-35</t>
+  </si>
+  <si>
+    <t>2013-03-05-17-23-14</t>
+  </si>
+  <si>
+    <t>2013-03-05-17-38-14</t>
+  </si>
+  <si>
+    <t>2013-03-05-17-43-55</t>
+  </si>
+  <si>
+    <t>2013-03-05-17-49-15</t>
+  </si>
+  <si>
+    <t>2013-03-05-17-55-29</t>
+  </si>
+  <si>
+    <t>2013-03-05-18-00-47</t>
+  </si>
+  <si>
+    <t>2013-03-05-18-06-33</t>
   </si>
 </sst>
 </file>
@@ -314,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,6 +377,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -626,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:A61"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2044,6 +2101,351 @@
         <v>24</v>
       </c>
       <c r="G61" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C62" s="3">
+        <v>41338</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G62" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C63" s="3">
+        <v>41338</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G63" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C64" s="3">
+        <v>41338</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G64" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C65" s="3">
+        <v>41338</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G65" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C66" s="3">
+        <v>41338</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G66" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C67" s="3">
+        <v>41338</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G67" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C68" s="3">
+        <v>41338</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G68" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C69" s="3">
+        <v>41338</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G69" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C70" s="3">
+        <v>41338</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G70" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C71" s="3">
+        <v>41338</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G71" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C72" s="3">
+        <v>41338</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G72" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C73" s="3">
+        <v>41338</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G73" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C74" s="3">
+        <v>41338</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G74" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C75" s="3">
+        <v>41338</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G75" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C76" s="3">
+        <v>41338</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G76" s="2">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more data analysis code
</commit_message>
<xml_diff>
--- a/dataAnalysisCodes/watchERP/01-preprocess-plot/watchErpDataset2.xlsx
+++ b/dataAnalysisCodes/watchERP/01-preprocess-plot/watchErpDataset2.xlsx
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1799,7 +1799,7 @@
         <v>69</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="G48" s="2">
         <v>1</v>
@@ -1937,7 +1937,7 @@
         <v>75</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="G54" s="2">
         <v>2</v>
@@ -1983,7 +1983,7 @@
         <v>77</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="G56" s="2">
         <v>3</v>

</xml_diff>

<commit_message>
added function for checciing status channel and eegs after recording
</commit_message>
<xml_diff>
--- a/dataAnalysisCodes/watchERP/01-preprocess-plot/watchErpDataset2.xlsx
+++ b/dataAnalysisCodes/watchERP/01-preprocess-plot/watchErpDataset2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="102">
   <si>
     <t>date</t>
   </si>
@@ -268,9 +268,6 @@
   </si>
   <si>
     <t>2013-03-04-nick</t>
-  </si>
-  <si>
-    <t>oddball.bdf</t>
   </si>
   <si>
     <t>S5</t>
@@ -685,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,19 +2103,19 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C62" s="3">
         <v>41338</v>
       </c>
       <c r="D62" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>45</v>
@@ -2129,19 +2126,19 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C63" s="3">
         <v>41338</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>24</v>
@@ -2152,19 +2149,19 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C64" s="3">
         <v>41338</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>45</v>
@@ -2175,22 +2172,22 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C65" s="3">
         <v>41338</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="G65" s="2">
         <v>1</v>
@@ -2198,19 +2195,19 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C66" s="3">
         <v>41338</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>47</v>
@@ -2221,19 +2218,19 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C67" s="3">
         <v>41338</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>44</v>
@@ -2244,19 +2241,19 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C68" s="3">
         <v>41338</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>44</v>
@@ -2267,22 +2264,22 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C69" s="3">
         <v>41338</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="G69" s="2">
         <v>2</v>
@@ -2290,19 +2287,19 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C70" s="3">
         <v>41338</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>47</v>
@@ -2313,19 +2310,19 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C71" s="3">
         <v>41338</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>45</v>
@@ -2336,22 +2333,22 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C72" s="3">
         <v>41338</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="G72" s="2">
         <v>3</v>
@@ -2359,19 +2356,19 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C73" s="3">
         <v>41338</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>44</v>
@@ -2382,19 +2379,19 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C74" s="3">
         <v>41338</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>24</v>
@@ -2405,19 +2402,19 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C75" s="3">
         <v>41338</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>24</v>
@@ -2428,19 +2425,19 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C76" s="3">
         <v>41338</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
bit of cleaning in 02-ter
</commit_message>
<xml_diff>
--- a/dataAnalysisCodes/watchERP/01-preprocess-plot/watchErpDataset2.xlsx
+++ b/dataAnalysisCodes/watchERP/01-preprocess-plot/watchErpDataset2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="120">
   <si>
     <t>date</t>
   </si>
@@ -322,6 +322,60 @@
   </si>
   <si>
     <t>2013-03-05-18-06-33</t>
+  </si>
+  <si>
+    <t>2013-03-25-anderson</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>2013-03-25-15-22-16</t>
+  </si>
+  <si>
+    <t>2013-03-25-15-38-39</t>
+  </si>
+  <si>
+    <t>2013-03-25-16-01-53</t>
+  </si>
+  <si>
+    <t>2013-03-25-16-09-13</t>
+  </si>
+  <si>
+    <t>2013-03-25-16-16-03</t>
+  </si>
+  <si>
+    <t>2013-03-25-16-25-57</t>
+  </si>
+  <si>
+    <t>2013-03-25-16-32-17</t>
+  </si>
+  <si>
+    <t>2013-03-25-16-38-06</t>
+  </si>
+  <si>
+    <t>2013-03-25-16-44-42</t>
+  </si>
+  <si>
+    <t>2013-03-25-16-50-37</t>
+  </si>
+  <si>
+    <t>2013-03-25-17-01-48</t>
+  </si>
+  <si>
+    <t>2013-03-25-17-07-53</t>
+  </si>
+  <si>
+    <t>2013-03-25-17-13-59</t>
+  </si>
+  <si>
+    <t>2013-03-25-17-21-29</t>
+  </si>
+  <si>
+    <t>2013-03-25-17-27-31</t>
   </si>
 </sst>
 </file>
@@ -680,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J91" sqref="J91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,7 +745,7 @@
     <col min="1" max="1" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4" style="2" bestFit="1" customWidth="1"/>
@@ -2443,6 +2497,351 @@
         <v>47</v>
       </c>
       <c r="G76" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C77" s="3">
+        <v>41358</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G77" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C78" s="3">
+        <v>41358</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G78" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C79" s="3">
+        <v>41358</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G79" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C80" s="3">
+        <v>41358</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G80" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C81" s="3">
+        <v>41358</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G81" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C82" s="3">
+        <v>41358</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G82" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C83" s="3">
+        <v>41358</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G83" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C84" s="3">
+        <v>41358</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G84" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C85" s="3">
+        <v>41358</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G85" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C86" s="3">
+        <v>41358</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G86" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C87" s="3">
+        <v>41358</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G87" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C88" s="3">
+        <v>41358</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G88" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C89" s="3">
+        <v>41358</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G89" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C90" s="3">
+        <v>41358</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G90" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C91" s="3">
+        <v>41358</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G91" s="2">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added some statistical analasys scripts and manuscript draft
</commit_message>
<xml_diff>
--- a/dataAnalysisCodes/watchERP/01-preprocess-plot/watchErpDataset2.xlsx
+++ b/dataAnalysisCodes/watchERP/01-preprocess-plot/watchErpDataset2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="139">
   <si>
     <t>date</t>
   </si>
@@ -376,6 +376,63 @@
   </si>
   <si>
     <t>2013-03-25-17-27-31</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>Elvira</t>
+  </si>
+  <si>
+    <t>2013-03-27-elvira</t>
+  </si>
+  <si>
+    <t>2013-03-27-15-10-32</t>
+  </si>
+  <si>
+    <t>2013-03-27-15-27-12</t>
+  </si>
+  <si>
+    <t>2013-03-27-15-34-15</t>
+  </si>
+  <si>
+    <t>2013-03-27-15-40-06</t>
+  </si>
+  <si>
+    <t>2013-03-27-15-45-54</t>
+  </si>
+  <si>
+    <t>2013-03-27-15-58-21</t>
+  </si>
+  <si>
+    <t>2013-03-27-16-04-13</t>
+  </si>
+  <si>
+    <t>2013-03-27-16-12-09</t>
+  </si>
+  <si>
+    <t>2013-03-27-16-20-10</t>
+  </si>
+  <si>
+    <t>2013-03-27-16-26-09</t>
+  </si>
+  <si>
+    <t>2013-03-27-16-44-22</t>
+  </si>
+  <si>
+    <t>2013-03-27-16-50-29</t>
+  </si>
+  <si>
+    <t>2013-03-27-16-56-34</t>
+  </si>
+  <si>
+    <t>2013-03-27-17-02-11</t>
+  </si>
+  <si>
+    <t>2013-03-27-17-08-36</t>
+  </si>
+  <si>
+    <t>frequency</t>
   </si>
 </sst>
 </file>
@@ -734,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J91" sqref="J91"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,11 +805,12 @@
     <col min="4" max="4" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -772,10 +830,13 @@
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -795,10 +856,13 @@
         <v>44</v>
       </c>
       <c r="G2" s="2">
+        <v>10</v>
+      </c>
+      <c r="H2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -818,10 +882,13 @@
         <v>45</v>
       </c>
       <c r="G3" s="2">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -841,10 +908,13 @@
         <v>46</v>
       </c>
       <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -864,10 +934,13 @@
         <v>45</v>
       </c>
       <c r="G5" s="2">
+        <v>15</v>
+      </c>
+      <c r="H5" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -887,10 +960,13 @@
         <v>47</v>
       </c>
       <c r="G6" s="2">
+        <v>12</v>
+      </c>
+      <c r="H6" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -910,10 +986,13 @@
         <v>47</v>
       </c>
       <c r="G7" s="2">
+        <v>12</v>
+      </c>
+      <c r="H7" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -933,10 +1012,13 @@
         <v>24</v>
       </c>
       <c r="G8" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H8" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -956,10 +1038,13 @@
         <v>47</v>
       </c>
       <c r="G9" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H9" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -979,10 +1064,13 @@
         <v>44</v>
       </c>
       <c r="G10" s="2">
+        <v>10</v>
+      </c>
+      <c r="H10" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -1002,10 +1090,13 @@
         <v>24</v>
       </c>
       <c r="G11" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H11" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -1025,10 +1116,13 @@
         <v>24</v>
       </c>
       <c r="G12" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8.57</v>
+      </c>
+      <c r="H12" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -1048,10 +1142,13 @@
         <v>45</v>
       </c>
       <c r="G13" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="H13" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -1071,10 +1168,13 @@
         <v>46</v>
       </c>
       <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1094,10 +1194,13 @@
         <v>44</v>
       </c>
       <c r="G15" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="H15" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
@@ -1117,10 +1220,13 @@
         <v>46</v>
       </c>
       <c r="G16" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -1140,10 +1246,13 @@
         <v>44</v>
       </c>
       <c r="G17" s="2">
+        <v>10</v>
+      </c>
+      <c r="H17" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -1163,10 +1272,13 @@
         <v>45</v>
       </c>
       <c r="G18" s="2">
+        <v>15</v>
+      </c>
+      <c r="H18" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
@@ -1186,10 +1298,13 @@
         <v>24</v>
       </c>
       <c r="G19" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H19" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
@@ -1209,10 +1324,13 @@
         <v>45</v>
       </c>
       <c r="G20" s="2">
+        <v>15</v>
+      </c>
+      <c r="H20" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
@@ -1232,10 +1350,13 @@
         <v>44</v>
       </c>
       <c r="G21" s="2">
+        <v>10</v>
+      </c>
+      <c r="H21" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1255,10 +1376,13 @@
         <v>46</v>
       </c>
       <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -1278,10 +1402,13 @@
         <v>46</v>
       </c>
       <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
@@ -1301,10 +1428,13 @@
         <v>47</v>
       </c>
       <c r="G24" s="2">
+        <v>12</v>
+      </c>
+      <c r="H24" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
@@ -1324,10 +1454,13 @@
         <v>47</v>
       </c>
       <c r="G25" s="2">
+        <v>12</v>
+      </c>
+      <c r="H25" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -1347,10 +1480,13 @@
         <v>46</v>
       </c>
       <c r="G26" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -1370,10 +1506,13 @@
         <v>24</v>
       </c>
       <c r="G27" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H27" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -1393,10 +1532,13 @@
         <v>47</v>
       </c>
       <c r="G28" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H28" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
@@ -1416,10 +1558,13 @@
         <v>24</v>
       </c>
       <c r="G29" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8.57</v>
+      </c>
+      <c r="H29" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
@@ -1439,10 +1584,13 @@
         <v>45</v>
       </c>
       <c r="G30" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="H30" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>26</v>
       </c>
@@ -1462,10 +1610,13 @@
         <v>44</v>
       </c>
       <c r="G31" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="H31" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>48</v>
       </c>
@@ -1485,10 +1636,13 @@
         <v>24</v>
       </c>
       <c r="G32" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H32" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>48</v>
       </c>
@@ -1508,10 +1662,13 @@
         <v>46</v>
       </c>
       <c r="G33" s="2">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>48</v>
       </c>
@@ -1531,10 +1688,13 @@
         <v>45</v>
       </c>
       <c r="G34" s="2">
+        <v>15</v>
+      </c>
+      <c r="H34" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>48</v>
       </c>
@@ -1554,10 +1714,13 @@
         <v>24</v>
       </c>
       <c r="G35" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H35" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>48</v>
       </c>
@@ -1577,10 +1740,13 @@
         <v>24</v>
       </c>
       <c r="G36" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8.57</v>
+      </c>
+      <c r="H36" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>48</v>
       </c>
@@ -1600,10 +1766,13 @@
         <v>44</v>
       </c>
       <c r="G37" s="2">
+        <v>10</v>
+      </c>
+      <c r="H37" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>48</v>
       </c>
@@ -1623,10 +1792,13 @@
         <v>47</v>
       </c>
       <c r="G38" s="2">
+        <v>12</v>
+      </c>
+      <c r="H38" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>48</v>
       </c>
@@ -1646,10 +1818,13 @@
         <v>47</v>
       </c>
       <c r="G39" s="2">
+        <v>12</v>
+      </c>
+      <c r="H39" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>48</v>
       </c>
@@ -1669,10 +1844,13 @@
         <v>46</v>
       </c>
       <c r="G40" s="2">
+        <v>0</v>
+      </c>
+      <c r="H40" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>48</v>
       </c>
@@ -1692,10 +1870,13 @@
         <v>45</v>
       </c>
       <c r="G41" s="2">
+        <v>15</v>
+      </c>
+      <c r="H41" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>48</v>
       </c>
@@ -1715,10 +1896,13 @@
         <v>47</v>
       </c>
       <c r="G42" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H42" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
@@ -1738,10 +1922,13 @@
         <v>45</v>
       </c>
       <c r="G43" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="H43" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>48</v>
       </c>
@@ -1761,10 +1948,13 @@
         <v>44</v>
       </c>
       <c r="G44" s="2">
+        <v>10</v>
+      </c>
+      <c r="H44" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>48</v>
       </c>
@@ -1784,10 +1974,13 @@
         <v>44</v>
       </c>
       <c r="G45" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="H45" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>48</v>
       </c>
@@ -1807,10 +2000,13 @@
         <v>46</v>
       </c>
       <c r="G46" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H46" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>66</v>
       </c>
@@ -1830,10 +2026,13 @@
         <v>44</v>
       </c>
       <c r="G47" s="2">
+        <v>10</v>
+      </c>
+      <c r="H47" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>66</v>
       </c>
@@ -1853,10 +2052,13 @@
         <v>46</v>
       </c>
       <c r="G48" s="2">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>66</v>
       </c>
@@ -1876,10 +2078,13 @@
         <v>47</v>
       </c>
       <c r="G49" s="2">
+        <v>12</v>
+      </c>
+      <c r="H49" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>66</v>
       </c>
@@ -1899,10 +2104,13 @@
         <v>44</v>
       </c>
       <c r="G50" s="2">
+        <v>10</v>
+      </c>
+      <c r="H50" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>66</v>
       </c>
@@ -1922,10 +2130,13 @@
         <v>45</v>
       </c>
       <c r="G51" s="2">
+        <v>15</v>
+      </c>
+      <c r="H51" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>66</v>
       </c>
@@ -1945,10 +2156,13 @@
         <v>44</v>
       </c>
       <c r="G52" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="H52" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>66</v>
       </c>
@@ -1968,10 +2182,13 @@
         <v>47</v>
       </c>
       <c r="G53" s="2">
+        <v>12</v>
+      </c>
+      <c r="H53" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>66</v>
       </c>
@@ -1991,10 +2208,13 @@
         <v>46</v>
       </c>
       <c r="G54" s="2">
+        <v>0</v>
+      </c>
+      <c r="H54" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>66</v>
       </c>
@@ -2014,10 +2234,13 @@
         <v>24</v>
       </c>
       <c r="G55" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H55" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>66</v>
       </c>
@@ -2037,10 +2260,13 @@
         <v>46</v>
       </c>
       <c r="G56" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H56" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>66</v>
       </c>
@@ -2060,10 +2286,13 @@
         <v>45</v>
       </c>
       <c r="G57" s="2">
+        <v>15</v>
+      </c>
+      <c r="H57" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>66</v>
       </c>
@@ -2083,10 +2312,13 @@
         <v>45</v>
       </c>
       <c r="G58" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="H58" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>66</v>
       </c>
@@ -2106,10 +2338,13 @@
         <v>24</v>
       </c>
       <c r="G59" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H59" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>66</v>
       </c>
@@ -2129,10 +2364,13 @@
         <v>47</v>
       </c>
       <c r="G60" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H60" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>66</v>
       </c>
@@ -2152,10 +2390,13 @@
         <v>24</v>
       </c>
       <c r="G61" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8.57</v>
+      </c>
+      <c r="H61" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>84</v>
       </c>
@@ -2175,10 +2416,13 @@
         <v>45</v>
       </c>
       <c r="G62" s="2">
+        <v>15</v>
+      </c>
+      <c r="H62" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>84</v>
       </c>
@@ -2198,10 +2442,13 @@
         <v>24</v>
       </c>
       <c r="G63" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H63" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>84</v>
       </c>
@@ -2221,10 +2468,13 @@
         <v>45</v>
       </c>
       <c r="G64" s="2">
+        <v>15</v>
+      </c>
+      <c r="H64" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>84</v>
       </c>
@@ -2244,10 +2494,13 @@
         <v>46</v>
       </c>
       <c r="G65" s="2">
+        <v>0</v>
+      </c>
+      <c r="H65" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>84</v>
       </c>
@@ -2267,10 +2520,13 @@
         <v>47</v>
       </c>
       <c r="G66" s="2">
+        <v>12</v>
+      </c>
+      <c r="H66" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>84</v>
       </c>
@@ -2290,10 +2546,13 @@
         <v>44</v>
       </c>
       <c r="G67" s="2">
+        <v>10</v>
+      </c>
+      <c r="H67" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>84</v>
       </c>
@@ -2313,10 +2572,13 @@
         <v>44</v>
       </c>
       <c r="G68" s="2">
+        <v>10</v>
+      </c>
+      <c r="H68" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>84</v>
       </c>
@@ -2336,10 +2598,13 @@
         <v>46</v>
       </c>
       <c r="G69" s="2">
+        <v>0</v>
+      </c>
+      <c r="H69" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>84</v>
       </c>
@@ -2359,10 +2624,13 @@
         <v>47</v>
       </c>
       <c r="G70" s="2">
+        <v>12</v>
+      </c>
+      <c r="H70" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>84</v>
       </c>
@@ -2382,10 +2650,13 @@
         <v>45</v>
       </c>
       <c r="G71" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="H71" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>84</v>
       </c>
@@ -2405,10 +2676,13 @@
         <v>46</v>
       </c>
       <c r="G72" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H72" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>84</v>
       </c>
@@ -2428,10 +2702,13 @@
         <v>44</v>
       </c>
       <c r="G73" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="H73" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>84</v>
       </c>
@@ -2451,10 +2728,13 @@
         <v>24</v>
       </c>
       <c r="G74" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H74" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>84</v>
       </c>
@@ -2474,10 +2754,13 @@
         <v>24</v>
       </c>
       <c r="G75" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8.57</v>
+      </c>
+      <c r="H75" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>84</v>
       </c>
@@ -2497,10 +2780,13 @@
         <v>47</v>
       </c>
       <c r="G76" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H76" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>103</v>
       </c>
@@ -2520,10 +2806,13 @@
         <v>24</v>
       </c>
       <c r="G77" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H77" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>103</v>
       </c>
@@ -2543,10 +2832,13 @@
         <v>44</v>
       </c>
       <c r="G78" s="2">
+        <v>10</v>
+      </c>
+      <c r="H78" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>103</v>
       </c>
@@ -2566,10 +2858,13 @@
         <v>47</v>
       </c>
       <c r="G79" s="2">
+        <v>12</v>
+      </c>
+      <c r="H79" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>103</v>
       </c>
@@ -2589,10 +2884,13 @@
         <v>45</v>
       </c>
       <c r="G80" s="2">
+        <v>15</v>
+      </c>
+      <c r="H80" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>103</v>
       </c>
@@ -2612,10 +2910,13 @@
         <v>46</v>
       </c>
       <c r="G81" s="2">
+        <v>0</v>
+      </c>
+      <c r="H81" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>103</v>
       </c>
@@ -2635,10 +2936,13 @@
         <v>46</v>
       </c>
       <c r="G82" s="2">
+        <v>0</v>
+      </c>
+      <c r="H82" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>103</v>
       </c>
@@ -2658,10 +2962,13 @@
         <v>44</v>
       </c>
       <c r="G83" s="2">
+        <v>10</v>
+      </c>
+      <c r="H83" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>103</v>
       </c>
@@ -2681,10 +2988,13 @@
         <v>47</v>
       </c>
       <c r="G84" s="2">
+        <v>12</v>
+      </c>
+      <c r="H84" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>103</v>
       </c>
@@ -2704,10 +3014,13 @@
         <v>45</v>
       </c>
       <c r="G85" s="2">
+        <v>15</v>
+      </c>
+      <c r="H85" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>103</v>
       </c>
@@ -2727,10 +3040,13 @@
         <v>24</v>
       </c>
       <c r="G86" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H86" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>103</v>
       </c>
@@ -2750,10 +3066,13 @@
         <v>47</v>
       </c>
       <c r="G87" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H87" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>103</v>
       </c>
@@ -2773,10 +3092,13 @@
         <v>45</v>
       </c>
       <c r="G88" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="H88" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>103</v>
       </c>
@@ -2796,10 +3118,13 @@
         <v>24</v>
       </c>
       <c r="G89" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8.57</v>
+      </c>
+      <c r="H89" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>103</v>
       </c>
@@ -2819,10 +3144,13 @@
         <v>46</v>
       </c>
       <c r="G90" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H90" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>103</v>
       </c>
@@ -2842,6 +3170,399 @@
         <v>44</v>
       </c>
       <c r="G91" s="2">
+        <v>10</v>
+      </c>
+      <c r="H91" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C92" s="3">
+        <v>41360</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G92" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H92" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C93" s="3">
+        <v>41360</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G93" s="2">
+        <v>10</v>
+      </c>
+      <c r="H93" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C94" s="3">
+        <v>41360</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G94" s="2">
+        <v>0</v>
+      </c>
+      <c r="H94" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C95" s="3">
+        <v>41360</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G95" s="2">
+        <v>12</v>
+      </c>
+      <c r="H95" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C96" s="3">
+        <v>41360</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G96" s="2">
+        <v>12</v>
+      </c>
+      <c r="H96" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C97" s="3">
+        <v>41360</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G97" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H97" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C98" s="3">
+        <v>41360</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G98" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H98" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C99" s="3">
+        <v>41360</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G99" s="2">
+        <v>10</v>
+      </c>
+      <c r="H99" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C100" s="3">
+        <v>41360</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G100" s="2">
+        <v>12</v>
+      </c>
+      <c r="H100" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C101" s="3">
+        <v>41360</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G101" s="2">
+        <v>15</v>
+      </c>
+      <c r="H101" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C102" s="3">
+        <v>41360</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G102" s="2">
+        <v>15</v>
+      </c>
+      <c r="H102" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C103" s="3">
+        <v>41360</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G103" s="2">
+        <v>10</v>
+      </c>
+      <c r="H103" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C104" s="3">
+        <v>41360</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G104" s="2">
+        <v>0</v>
+      </c>
+      <c r="H104" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C105" s="3">
+        <v>41360</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G105" s="2">
+        <v>0</v>
+      </c>
+      <c r="H105" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C106" s="3">
+        <v>41360</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G106" s="2">
+        <v>15</v>
+      </c>
+      <c r="H106" s="2">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
plenty of new stuffs - before neufchateau
</commit_message>
<xml_diff>
--- a/dataAnalysisCodes/watchERP/01-preprocess-plot/watchErpDataset2.xlsx
+++ b/dataAnalysisCodes/watchERP/01-preprocess-plot/watchErpDataset2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="175">
   <si>
     <t>date</t>
   </si>
@@ -487,6 +487,60 @@
   </si>
   <si>
     <t>2013-04-11-16-31-22</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>Alejandro</t>
+  </si>
+  <si>
+    <t>2013-07-02-alejandro</t>
+  </si>
+  <si>
+    <t>2013-07-02-10-41-52</t>
+  </si>
+  <si>
+    <t>2013-07-02-10-51-04</t>
+  </si>
+  <si>
+    <t>2013-07-02-10-58-51</t>
+  </si>
+  <si>
+    <t>2013-07-02-11-05-55</t>
+  </si>
+  <si>
+    <t>2013-07-02-11-14-05</t>
+  </si>
+  <si>
+    <t>2013-07-02-11-37-37</t>
+  </si>
+  <si>
+    <t>2013-07-02-11-45-28</t>
+  </si>
+  <si>
+    <t>2013-07-02-11-52-29</t>
+  </si>
+  <si>
+    <t>2013-07-02-11-59-14</t>
+  </si>
+  <si>
+    <t>2013-07-02-12-06-08</t>
+  </si>
+  <si>
+    <t>2013-07-02-12-18-34</t>
+  </si>
+  <si>
+    <t>2013-07-02-12-24-49</t>
+  </si>
+  <si>
+    <t>2013-07-02-12-31-13</t>
+  </si>
+  <si>
+    <t>2013-07-02-12-37-25</t>
+  </si>
+  <si>
+    <t>2013-07-02-12-43-59</t>
   </si>
 </sst>
 </file>
@@ -845,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H121"/>
+  <dimension ref="A1:H136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108:A121"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4007,6 +4061,396 @@
         <v>10</v>
       </c>
       <c r="H121" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C122" s="3">
+        <v>41457</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G122" s="2">
+        <v>0</v>
+      </c>
+      <c r="H122" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C123" s="3">
+        <v>41457</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G123" s="2">
+        <v>12</v>
+      </c>
+      <c r="H123" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C124" s="3">
+        <v>41457</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G124" s="2">
+        <v>12</v>
+      </c>
+      <c r="H124" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C125" s="3">
+        <v>41457</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G125" s="2">
+        <v>0</v>
+      </c>
+      <c r="H125" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C126" s="3">
+        <v>41457</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G126" s="2">
+        <v>15</v>
+      </c>
+      <c r="H126" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C127" s="3">
+        <v>41457</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G127" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H127" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C128" s="3">
+        <v>41457</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G128" s="2">
+        <v>10</v>
+      </c>
+      <c r="H128" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C129" s="3">
+        <v>41457</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G129" s="2">
+        <v>0</v>
+      </c>
+      <c r="H129" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C130" s="3">
+        <v>41457</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G130" s="2">
+        <v>15</v>
+      </c>
+      <c r="H130" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C131" s="3">
+        <v>41457</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G131" s="2">
+        <v>10</v>
+      </c>
+      <c r="H131" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C132" s="3">
+        <v>41457</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G132" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H132" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C133" s="3">
+        <v>41457</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G133" s="2">
+        <v>10</v>
+      </c>
+      <c r="H133" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C134" s="3">
+        <v>41457</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G134" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H134" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C135" s="3">
+        <v>41457</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G135" s="2">
+        <v>15</v>
+      </c>
+      <c r="H135" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C136" s="3">
+        <v>41457</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G136" s="2">
+        <v>12</v>
+      </c>
+      <c r="H136" s="2">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
not much to say
</commit_message>
<xml_diff>
--- a/dataAnalysisCodes/watchERP/01-preprocess-plot/watchErpDataset2.xlsx
+++ b/dataAnalysisCodes/watchERP/01-preprocess-plot/watchErpDataset2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="193">
   <si>
     <t>date</t>
   </si>
@@ -27,9 +27,6 @@
     <t>run</t>
   </si>
   <si>
-    <t>S1</t>
-  </si>
-  <si>
     <t>Adrien</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>2013-02-25-adrien</t>
   </si>
   <si>
-    <t>S2</t>
-  </si>
-  <si>
     <t>2013-02-26-nikolay</t>
   </si>
   <si>
@@ -162,9 +156,6 @@
     <t>hybrid-12Hz</t>
   </si>
   <si>
-    <t>S3</t>
-  </si>
-  <si>
     <t>Marijn</t>
   </si>
   <si>
@@ -216,9 +207,6 @@
     <t>2013-02-28-marijn</t>
   </si>
   <si>
-    <t>S4</t>
-  </si>
-  <si>
     <t>Nick</t>
   </si>
   <si>
@@ -270,9 +258,6 @@
     <t>2013-03-04-nick</t>
   </si>
   <si>
-    <t>S5</t>
-  </si>
-  <si>
     <t>Jaime</t>
   </si>
   <si>
@@ -327,9 +312,6 @@
     <t>2013-03-25-anderson</t>
   </si>
   <si>
-    <t>S6</t>
-  </si>
-  <si>
     <t>Anderson</t>
   </si>
   <si>
@@ -378,9 +360,6 @@
     <t>2013-03-25-17-27-31</t>
   </si>
   <si>
-    <t>S7</t>
-  </si>
-  <si>
     <t>Elvira</t>
   </si>
   <si>
@@ -435,9 +414,6 @@
     <t>frequency</t>
   </si>
   <si>
-    <t>S8</t>
-  </si>
-  <si>
     <t>Robert</t>
   </si>
   <si>
@@ -489,9 +465,6 @@
     <t>2013-04-11-16-31-22</t>
   </si>
   <si>
-    <t>S9</t>
-  </si>
-  <si>
     <t>Alejandro</t>
   </si>
   <si>
@@ -541,6 +514,87 @@
   </si>
   <si>
     <t>2013-07-02-12-43-59</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>Yelena</t>
+  </si>
+  <si>
+    <t>2013-07-19-yelena</t>
+  </si>
+  <si>
+    <t>2013-07-19-15-51-15</t>
+  </si>
+  <si>
+    <t>2013-07-19-15-59-03</t>
+  </si>
+  <si>
+    <t>2013-07-19-16-06-52</t>
+  </si>
+  <si>
+    <t>2013-07-19-16-13-41</t>
+  </si>
+  <si>
+    <t>2013-07-19-16-22-46</t>
+  </si>
+  <si>
+    <t>2013-07-19-16-37-56</t>
+  </si>
+  <si>
+    <t>2013-07-19-16-44-40</t>
+  </si>
+  <si>
+    <t>2013-07-19-16-51-56</t>
+  </si>
+  <si>
+    <t>2013-07-19-16-58-04</t>
+  </si>
+  <si>
+    <t>2013-07-19-17-05-22</t>
+  </si>
+  <si>
+    <t>2013-07-19-17-21-47</t>
+  </si>
+  <si>
+    <t>2013-07-19-17-28-13</t>
+  </si>
+  <si>
+    <t>2013-07-19-17-35-52</t>
+  </si>
+  <si>
+    <t>2013-07-19-17-42-30</t>
+  </si>
+  <si>
+    <t>2013-07-19-17-58-42</t>
+  </si>
+  <si>
+    <t>S01</t>
+  </si>
+  <si>
+    <t>S02</t>
+  </si>
+  <si>
+    <t>S03</t>
+  </si>
+  <si>
+    <t>S04</t>
+  </si>
+  <si>
+    <t>S05</t>
+  </si>
+  <si>
+    <t>S06</t>
+  </si>
+  <si>
+    <t>S07</t>
+  </si>
+  <si>
+    <t>S08</t>
+  </si>
+  <si>
+    <t>S09</t>
   </si>
 </sst>
 </file>
@@ -899,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H136"/>
+  <dimension ref="A1:H151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K120" sqref="K120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,25 +974,25 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
@@ -946,22 +1000,22 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3">
         <v>41330</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G2" s="2">
         <v>10</v>
@@ -972,22 +1026,22 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3">
         <v>41330</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G3" s="2">
         <v>15</v>
@@ -998,22 +1052,22 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3">
         <v>41330</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
@@ -1024,22 +1078,22 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="3">
         <v>41330</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G5" s="2">
         <v>15</v>
@@ -1050,22 +1104,22 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="3">
         <v>41330</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G6" s="2">
         <v>12</v>
@@ -1076,22 +1130,22 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3">
         <v>41330</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G7" s="2">
         <v>12</v>
@@ -1102,22 +1156,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="3">
         <v>41330</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G8" s="2">
         <v>8.57</v>
@@ -1128,22 +1182,22 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="3">
         <v>41330</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G9" s="2">
         <v>12</v>
@@ -1154,22 +1208,22 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="3">
         <v>41330</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G10" s="2">
         <v>10</v>
@@ -1180,22 +1234,22 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="3">
         <v>41330</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" s="2">
         <v>8.57</v>
@@ -1206,22 +1260,22 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="3">
         <v>41330</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12" s="2">
         <v>8.57</v>
@@ -1232,22 +1286,22 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="3">
         <v>41330</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G13" s="2">
         <v>15</v>
@@ -1258,22 +1312,22 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="3">
         <v>41330</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G14" s="2">
         <v>0</v>
@@ -1284,22 +1338,22 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15" s="3">
         <v>41330</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G15" s="2">
         <v>10</v>
@@ -1310,22 +1364,22 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" s="3">
         <v>41330</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G16" s="2">
         <v>0</v>
@@ -1336,22 +1390,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C17" s="3">
         <v>41331</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G17" s="2">
         <v>10</v>
@@ -1362,22 +1416,22 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C18" s="3">
         <v>41331</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G18" s="2">
         <v>15</v>
@@ -1388,22 +1442,22 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C19" s="3">
         <v>41331</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G19" s="2">
         <v>8.57</v>
@@ -1414,22 +1468,22 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C20" s="3">
         <v>41331</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G20" s="2">
         <v>15</v>
@@ -1440,22 +1494,22 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C21" s="3">
         <v>41331</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G21" s="2">
         <v>10</v>
@@ -1466,22 +1520,22 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C22" s="3">
         <v>41331</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G22" s="2">
         <v>0</v>
@@ -1492,22 +1546,22 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C23" s="3">
         <v>41331</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G23" s="2">
         <v>0</v>
@@ -1518,22 +1572,22 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C24" s="3">
         <v>41331</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G24" s="2">
         <v>12</v>
@@ -1544,22 +1598,22 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C25" s="3">
         <v>41331</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G25" s="2">
         <v>12</v>
@@ -1570,22 +1624,22 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C26" s="3">
         <v>41331</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G26" s="2">
         <v>0</v>
@@ -1596,22 +1650,22 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C27" s="3">
         <v>41331</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G27" s="2">
         <v>8.57</v>
@@ -1622,22 +1676,22 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C28" s="3">
         <v>41331</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G28" s="2">
         <v>12</v>
@@ -1648,22 +1702,22 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C29" s="3">
         <v>41331</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G29" s="2">
         <v>8.57</v>
@@ -1674,22 +1728,22 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C30" s="3">
         <v>41331</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G30" s="2">
         <v>15</v>
@@ -1700,22 +1754,22 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C31" s="3">
         <v>41331</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G31" s="2">
         <v>10</v>
@@ -1726,22 +1780,22 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C32" s="3">
         <v>41333</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G32" s="2">
         <v>8.57</v>
@@ -1752,22 +1806,22 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C33" s="3">
         <v>41333</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G33" s="2">
         <v>0</v>
@@ -1778,22 +1832,22 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C34" s="3">
         <v>41333</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G34" s="2">
         <v>15</v>
@@ -1804,22 +1858,22 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C35" s="3">
         <v>41333</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G35" s="2">
         <v>8.57</v>
@@ -1830,22 +1884,22 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C36" s="3">
         <v>41333</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G36" s="2">
         <v>8.57</v>
@@ -1856,22 +1910,22 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C37" s="3">
         <v>41333</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G37" s="2">
         <v>10</v>
@@ -1882,22 +1936,22 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C38" s="3">
         <v>41333</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G38" s="2">
         <v>12</v>
@@ -1908,22 +1962,22 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C39" s="3">
         <v>41333</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G39" s="2">
         <v>12</v>
@@ -1934,22 +1988,22 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C40" s="3">
         <v>41333</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G40" s="2">
         <v>0</v>
@@ -1960,22 +2014,22 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C41" s="3">
         <v>41333</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G41" s="2">
         <v>15</v>
@@ -1986,22 +2040,22 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C42" s="3">
         <v>41333</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G42" s="2">
         <v>12</v>
@@ -2012,22 +2066,22 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C43" s="3">
         <v>41333</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G43" s="2">
         <v>15</v>
@@ -2038,22 +2092,22 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C44" s="3">
         <v>41333</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G44" s="2">
         <v>10</v>
@@ -2064,22 +2118,22 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C45" s="3">
         <v>41333</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G45" s="2">
         <v>10</v>
@@ -2090,22 +2144,22 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C46" s="3">
         <v>41333</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G46" s="2">
         <v>0</v>
@@ -2116,22 +2170,22 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>66</v>
+        <v>187</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C47" s="3">
         <v>41337</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G47" s="2">
         <v>10</v>
@@ -2142,22 +2196,22 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>66</v>
+        <v>187</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C48" s="3">
         <v>41337</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G48" s="2">
         <v>0</v>
@@ -2168,22 +2222,22 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>66</v>
+        <v>187</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C49" s="3">
         <v>41337</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G49" s="2">
         <v>12</v>
@@ -2194,22 +2248,22 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>66</v>
+        <v>187</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C50" s="3">
         <v>41337</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G50" s="2">
         <v>10</v>
@@ -2220,22 +2274,22 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>66</v>
+        <v>187</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C51" s="3">
         <v>41337</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G51" s="2">
         <v>15</v>
@@ -2246,22 +2300,22 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>66</v>
+        <v>187</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C52" s="3">
         <v>41337</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G52" s="2">
         <v>10</v>
@@ -2272,22 +2326,22 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>66</v>
+        <v>187</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C53" s="3">
         <v>41337</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G53" s="2">
         <v>12</v>
@@ -2298,22 +2352,22 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>66</v>
+        <v>187</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C54" s="3">
         <v>41337</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G54" s="2">
         <v>0</v>
@@ -2324,22 +2378,22 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>66</v>
+        <v>187</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C55" s="3">
         <v>41337</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G55" s="2">
         <v>8.57</v>
@@ -2350,22 +2404,22 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>66</v>
+        <v>187</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C56" s="3">
         <v>41337</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G56" s="2">
         <v>0</v>
@@ -2376,22 +2430,22 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>66</v>
+        <v>187</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C57" s="3">
         <v>41337</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G57" s="2">
         <v>15</v>
@@ -2402,22 +2456,22 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>66</v>
+        <v>187</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C58" s="3">
         <v>41337</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G58" s="2">
         <v>15</v>
@@ -2428,22 +2482,22 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>66</v>
+        <v>187</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C59" s="3">
         <v>41337</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G59" s="2">
         <v>8.57</v>
@@ -2454,22 +2508,22 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>66</v>
+        <v>187</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C60" s="3">
         <v>41337</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G60" s="2">
         <v>12</v>
@@ -2480,22 +2534,22 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>66</v>
+        <v>187</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C61" s="3">
         <v>41337</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G61" s="2">
         <v>8.57</v>
@@ -2506,22 +2560,22 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C62" s="3">
         <v>41338</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G62" s="2">
         <v>15</v>
@@ -2532,22 +2586,22 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C63" s="3">
         <v>41338</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G63" s="2">
         <v>8.57</v>
@@ -2558,22 +2612,22 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C64" s="3">
         <v>41338</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G64" s="2">
         <v>15</v>
@@ -2584,22 +2638,22 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C65" s="3">
         <v>41338</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G65" s="2">
         <v>0</v>
@@ -2610,22 +2664,22 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C66" s="3">
         <v>41338</v>
       </c>
       <c r="D66" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E66" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E66" s="4" t="s">
-        <v>91</v>
-      </c>
       <c r="F66" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G66" s="2">
         <v>12</v>
@@ -2636,22 +2690,22 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C67" s="3">
         <v>41338</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G67" s="2">
         <v>10</v>
@@ -2662,22 +2716,22 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C68" s="3">
         <v>41338</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G68" s="2">
         <v>10</v>
@@ -2688,22 +2742,22 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C69" s="3">
         <v>41338</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G69" s="2">
         <v>0</v>
@@ -2714,22 +2768,22 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C70" s="3">
         <v>41338</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G70" s="2">
         <v>12</v>
@@ -2740,22 +2794,22 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C71" s="3">
         <v>41338</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G71" s="2">
         <v>15</v>
@@ -2766,22 +2820,22 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C72" s="3">
         <v>41338</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G72" s="2">
         <v>0</v>
@@ -2792,22 +2846,22 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C73" s="3">
         <v>41338</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G73" s="2">
         <v>10</v>
@@ -2818,22 +2872,22 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C74" s="3">
         <v>41338</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G74" s="2">
         <v>8.57</v>
@@ -2844,22 +2898,22 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C75" s="3">
         <v>41338</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G75" s="2">
         <v>8.57</v>
@@ -2870,22 +2924,22 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C76" s="3">
         <v>41338</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G76" s="2">
         <v>12</v>
@@ -2896,22 +2950,22 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C77" s="3">
         <v>41358</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G77" s="2">
         <v>8.57</v>
@@ -2922,22 +2976,22 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C78" s="3">
         <v>41358</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G78" s="2">
         <v>10</v>
@@ -2948,22 +3002,22 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C79" s="3">
         <v>41358</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G79" s="2">
         <v>12</v>
@@ -2974,22 +3028,22 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C80" s="3">
         <v>41358</v>
       </c>
       <c r="D80" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E80" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E80" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="F80" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G80" s="2">
         <v>15</v>
@@ -3000,22 +3054,22 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C81" s="3">
         <v>41358</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G81" s="2">
         <v>0</v>
@@ -3026,22 +3080,22 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C82" s="3">
         <v>41358</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G82" s="2">
         <v>0</v>
@@ -3052,22 +3106,22 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C83" s="3">
         <v>41358</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G83" s="2">
         <v>10</v>
@@ -3078,22 +3132,22 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C84" s="3">
         <v>41358</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G84" s="2">
         <v>12</v>
@@ -3104,22 +3158,22 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C85" s="3">
         <v>41358</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G85" s="2">
         <v>15</v>
@@ -3130,22 +3184,22 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C86" s="3">
         <v>41358</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G86" s="2">
         <v>8.57</v>
@@ -3156,22 +3210,22 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C87" s="3">
         <v>41358</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G87" s="2">
         <v>12</v>
@@ -3182,22 +3236,22 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C88" s="3">
         <v>41358</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G88" s="2">
         <v>15</v>
@@ -3208,22 +3262,22 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C89" s="3">
         <v>41358</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G89" s="2">
         <v>8.57</v>
@@ -3234,22 +3288,22 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C90" s="3">
         <v>41358</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G90" s="2">
         <v>0</v>
@@ -3260,22 +3314,22 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C91" s="3">
         <v>41358</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G91" s="2">
         <v>10</v>
@@ -3286,22 +3340,22 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C92" s="3">
         <v>41360</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G92" s="2">
         <v>8.57</v>
@@ -3312,22 +3366,22 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C93" s="3">
         <v>41360</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G93" s="2">
         <v>10</v>
@@ -3338,22 +3392,22 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C94" s="3">
         <v>41360</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G94" s="2">
         <v>0</v>
@@ -3364,22 +3418,22 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C95" s="3">
         <v>41360</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G95" s="2">
         <v>12</v>
@@ -3390,22 +3444,22 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C96" s="3">
         <v>41360</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G96" s="2">
         <v>12</v>
@@ -3416,22 +3470,22 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C97" s="3">
         <v>41360</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G97" s="2">
         <v>8.57</v>
@@ -3442,22 +3496,22 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C98" s="3">
         <v>41360</v>
       </c>
       <c r="D98" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E98" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E98" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="F98" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G98" s="2">
         <v>8.57</v>
@@ -3468,22 +3522,22 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C99" s="3">
         <v>41360</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G99" s="2">
         <v>10</v>
@@ -3494,22 +3548,22 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C100" s="3">
         <v>41360</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G100" s="2">
         <v>12</v>
@@ -3520,22 +3574,22 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C101" s="3">
         <v>41360</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G101" s="2">
         <v>15</v>
@@ -3546,22 +3600,22 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C102" s="3">
         <v>41360</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G102" s="2">
         <v>15</v>
@@ -3572,22 +3626,22 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C103" s="3">
         <v>41360</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G103" s="2">
         <v>10</v>
@@ -3598,22 +3652,22 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C104" s="3">
         <v>41360</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G104" s="2">
         <v>0</v>
@@ -3624,22 +3678,22 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C105" s="3">
         <v>41360</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G105" s="2">
         <v>0</v>
@@ -3650,22 +3704,22 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C106" s="3">
         <v>41360</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G106" s="2">
         <v>15</v>
@@ -3676,22 +3730,22 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C107" s="3">
         <v>41375</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G107" s="2">
         <v>12</v>
@@ -3702,22 +3756,22 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C108" s="3">
         <v>41375</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G108" s="2">
         <v>0</v>
@@ -3728,22 +3782,22 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C109" s="3">
         <v>41375</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G109" s="2">
         <v>10</v>
@@ -3754,22 +3808,22 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C110" s="3">
         <v>41375</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G110" s="2">
         <v>0</v>
@@ -3780,22 +3834,22 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C111" s="3">
         <v>41375</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G111" s="2">
         <v>15</v>
@@ -3806,22 +3860,22 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C112" s="3">
         <v>41375</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G112" s="2">
         <v>15</v>
@@ -3832,22 +3886,22 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C113" s="3">
         <v>41375</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G113" s="2">
         <v>8.57</v>
@@ -3858,22 +3912,22 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C114" s="3">
         <v>41375</v>
       </c>
       <c r="D114" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E114" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E114" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="F114" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G114" s="2">
         <v>12</v>
@@ -3884,22 +3938,22 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C115" s="3">
         <v>41375</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G115" s="2">
         <v>0</v>
@@ -3910,22 +3964,22 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C116" s="3">
         <v>41375</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G116" s="2">
         <v>10</v>
@@ -3936,22 +3990,22 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C117" s="3">
         <v>41375</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G117" s="2">
         <v>15</v>
@@ -3962,22 +4016,22 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C118" s="3">
         <v>41375</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G118" s="2">
         <v>12</v>
@@ -3988,22 +4042,22 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C119" s="3">
         <v>41375</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G119" s="2">
         <v>8.57</v>
@@ -4014,22 +4068,22 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C120" s="3">
         <v>41375</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G120" s="2">
         <v>8.57</v>
@@ -4040,22 +4094,22 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C121" s="3">
         <v>41375</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G121" s="2">
         <v>10</v>
@@ -4066,22 +4120,22 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C122" s="3">
         <v>41457</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G122" s="2">
         <v>0</v>
@@ -4092,22 +4146,22 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C123" s="3">
         <v>41457</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G123" s="2">
         <v>12</v>
@@ -4118,22 +4172,22 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C124" s="3">
         <v>41457</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G124" s="2">
         <v>12</v>
@@ -4144,22 +4198,22 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C125" s="3">
         <v>41457</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G125" s="2">
         <v>0</v>
@@ -4170,22 +4224,22 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C126" s="3">
         <v>41457</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G126" s="2">
         <v>15</v>
@@ -4196,22 +4250,22 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C127" s="3">
         <v>41457</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G127" s="2">
         <v>8.57</v>
@@ -4222,22 +4276,22 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C128" s="3">
         <v>41457</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G128" s="2">
         <v>10</v>
@@ -4248,22 +4302,22 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C129" s="3">
         <v>41457</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G129" s="2">
         <v>0</v>
@@ -4274,22 +4328,22 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C130" s="3">
         <v>41457</v>
       </c>
       <c r="D130" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E130" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E130" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="F130" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G130" s="2">
         <v>15</v>
@@ -4300,22 +4354,22 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C131" s="3">
         <v>41457</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G131" s="2">
         <v>10</v>
@@ -4326,22 +4380,22 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C132" s="3">
         <v>41457</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G132" s="2">
         <v>8.57</v>
@@ -4352,22 +4406,22 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C133" s="3">
         <v>41457</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G133" s="2">
         <v>10</v>
@@ -4378,22 +4432,22 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C134" s="3">
         <v>41457</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G134" s="2">
         <v>8.57</v>
@@ -4404,22 +4458,22 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C135" s="3">
         <v>41457</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G135" s="2">
         <v>15</v>
@@ -4430,27 +4484,417 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C136" s="3">
         <v>41457</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G136" s="2">
         <v>12</v>
       </c>
       <c r="H136" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C137" s="3">
+        <v>41474</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G137" s="2">
+        <v>12</v>
+      </c>
+      <c r="H137" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C138" s="3">
+        <v>41474</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G138" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H138" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C139" s="3">
+        <v>41474</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G139" s="2">
+        <v>0</v>
+      </c>
+      <c r="H139" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C140" s="3">
+        <v>41474</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G140" s="2">
+        <v>0</v>
+      </c>
+      <c r="H140" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C141" s="3">
+        <v>41474</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G141" s="2">
+        <v>10</v>
+      </c>
+      <c r="H141" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C142" s="3">
+        <v>41474</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G142" s="2">
+        <v>10</v>
+      </c>
+      <c r="H142" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C143" s="3">
+        <v>41474</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G143" s="2">
+        <v>15</v>
+      </c>
+      <c r="H143" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C144" s="3">
+        <v>41474</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G144" s="2">
+        <v>15</v>
+      </c>
+      <c r="H144" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C145" s="3">
+        <v>41474</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G145" s="2">
+        <v>12</v>
+      </c>
+      <c r="H145" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C146" s="3">
+        <v>41474</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G146" s="2">
+        <v>10</v>
+      </c>
+      <c r="H146" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C147" s="3">
+        <v>41474</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G147" s="2">
+        <v>15</v>
+      </c>
+      <c r="H147" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C148" s="3">
+        <v>41474</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G148" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H148" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C149" s="3">
+        <v>41474</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G149" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H149" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C150" s="3">
+        <v>41474</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G150" s="2">
+        <v>0</v>
+      </c>
+      <c r="H150" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C151" s="3">
+        <v>41474</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G151" s="2">
+        <v>12</v>
+      </c>
+      <c r="H151" s="2">
         <v>3</v>
       </c>
     </row>

</xml_diff>